<commit_message>
Updated WiFly Message IDs
</commit_message>
<xml_diff>
--- a/Documentation/WiFly Message IDs.xlsx
+++ b/Documentation/WiFly Message IDs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Message Type</t>
   </si>
@@ -32,67 +32,76 @@
     <t>ID</t>
   </si>
   <si>
-    <t>IR00</t>
-  </si>
-  <si>
-    <t>0x00</t>
-  </si>
-  <si>
-    <t>IR01</t>
-  </si>
-  <si>
-    <t>0x01</t>
-  </si>
-  <si>
-    <t>IR10</t>
-  </si>
-  <si>
     <t>0x10</t>
   </si>
   <si>
-    <t>IR11</t>
-  </si>
-  <si>
     <t>0x11</t>
   </si>
   <si>
-    <t>IR20</t>
-  </si>
-  <si>
-    <t>0x20</t>
-  </si>
-  <si>
-    <t>IR21</t>
-  </si>
-  <si>
-    <t>0x21</t>
-  </si>
-  <si>
-    <t>IR30</t>
-  </si>
-  <si>
-    <t>0x30</t>
-  </si>
-  <si>
-    <t>IR31</t>
-  </si>
-  <si>
-    <t>0x31</t>
-  </si>
-  <si>
-    <t>IR40</t>
-  </si>
-  <si>
-    <t>0x40</t>
-  </si>
-  <si>
-    <t>IR41</t>
-  </si>
-  <si>
-    <t>0x41</t>
-  </si>
-  <si>
     <t>ACK</t>
+  </si>
+  <si>
+    <t>0x99</t>
+  </si>
+  <si>
+    <t>MOTOR</t>
+  </si>
+  <si>
+    <t>0x50</t>
+  </si>
+  <si>
+    <t>IR1</t>
+  </si>
+  <si>
+    <t>IR2</t>
+  </si>
+  <si>
+    <t>IR3</t>
+  </si>
+  <si>
+    <t>IR0</t>
+  </si>
+  <si>
+    <t>IR4</t>
+  </si>
+  <si>
+    <t>IR5</t>
+  </si>
+  <si>
+    <t>IR6</t>
+  </si>
+  <si>
+    <t>IR7</t>
+  </si>
+  <si>
+    <t>IR8</t>
+  </si>
+  <si>
+    <t>IR9</t>
+  </si>
+  <si>
+    <t>0x12</t>
+  </si>
+  <si>
+    <t>0x13</t>
+  </si>
+  <si>
+    <t>0x14</t>
+  </si>
+  <si>
+    <t>0x15</t>
+  </si>
+  <si>
+    <t>0x16</t>
+  </si>
+  <si>
+    <t>0x17</t>
+  </si>
+  <si>
+    <t>0x18</t>
+  </si>
+  <si>
+    <t>0x19</t>
   </si>
 </sst>
 </file>
@@ -419,15 +428,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -440,50 +449,50 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -491,39 +500,47 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12">
-        <v>255</v>
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
back up to date
</commit_message>
<xml_diff>
--- a/Documentation/WiFly Message IDs.xlsx
+++ b/Documentation/WiFly Message IDs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Message Type</t>
   </si>
@@ -32,24 +32,12 @@
     <t>ID</t>
   </si>
   <si>
-    <t>0x10</t>
-  </si>
-  <si>
-    <t>0x11</t>
-  </si>
-  <si>
     <t>ACK</t>
   </si>
   <si>
-    <t>0x99</t>
-  </si>
-  <si>
     <t>MOTOR</t>
   </si>
   <si>
-    <t>0x50</t>
-  </si>
-  <si>
     <t>IR1</t>
   </si>
   <si>
@@ -78,30 +66,6 @@
   </si>
   <si>
     <t>IR9</t>
-  </si>
-  <si>
-    <t>0x12</t>
-  </si>
-  <si>
-    <t>0x13</t>
-  </si>
-  <si>
-    <t>0x14</t>
-  </si>
-  <si>
-    <t>0x15</t>
-  </si>
-  <si>
-    <t>0x16</t>
-  </si>
-  <si>
-    <t>0x17</t>
-  </si>
-  <si>
-    <t>0x18</t>
-  </si>
-  <si>
-    <t>0x19</t>
   </si>
 </sst>
 </file>
@@ -431,7 +395,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,98 +413,98 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>21</v>
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated WiFly Message Format
</commit_message>
<xml_diff>
--- a/Documentation/WiFly Message IDs.xlsx
+++ b/Documentation/WiFly Message IDs.xlsx
@@ -24,48 +24,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Message Type</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>ACK</t>
   </si>
   <si>
     <t>MOTOR</t>
   </si>
   <si>
-    <t>IR1</t>
-  </si>
-  <si>
-    <t>IR2</t>
-  </si>
-  <si>
-    <t>IR3</t>
-  </si>
-  <si>
-    <t>IR0</t>
-  </si>
-  <si>
-    <t>IR4</t>
-  </si>
-  <si>
-    <t>IR5</t>
-  </si>
-  <si>
-    <t>IR6</t>
-  </si>
-  <si>
-    <t>IR7</t>
-  </si>
-  <si>
-    <t>IR8</t>
-  </si>
-  <si>
-    <t>IR9</t>
+    <t>ID (Decimal)</t>
+  </si>
+  <si>
+    <t>Payload Length</t>
+  </si>
+  <si>
+    <t>SENSOR</t>
+  </si>
+  <si>
+    <t>Message Index #</t>
+  </si>
+  <si>
+    <t>Message Type ID</t>
+  </si>
+  <si>
+    <t>Payload</t>
+  </si>
+  <si>
+    <t>Terminator</t>
   </si>
 </sst>
 </file>
@@ -89,12 +77,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -109,9 +121,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,119 +408,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
+      <c r="C2">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>11</v>
+        <v>50</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13">
         <v>99</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated ACK payload length
</commit_message>
<xml_diff>
--- a/Documentation/WiFly Message IDs.xlsx
+++ b/Documentation/WiFly Message IDs.xlsx
@@ -411,7 +411,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,7 +479,7 @@
         <v>99</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>